<commit_message>
Added new columns to projects list, finished requests functinality
</commit_message>
<xml_diff>
--- a/database/Projects_List.xlsx
+++ b/database/Projects_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\FYP system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/advait/Desktop/gitpositories/sc2002/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFD87BB-8C6E-4C84-B41F-CD3CA9695C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76BC3F5-0D6C-1141-9A5C-C2F959BFD1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10700" yWindow="5520" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>Supervisor</t>
   </si>
@@ -112,13 +112,28 @@
   </si>
   <si>
     <t>Graph-based Deep Models for Image Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>ReplacementSupervisor</t>
+  </si>
+  <si>
+    <t>AVAILABLE</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,17 +142,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="64"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color indexed="64"/>
       <name val="Microsoft Sans Serif"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="64"/>
-      <name val="Microsoft Sans Serif"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,10 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,152 +468,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="74.44140625" customWidth="1"/>
+    <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Covered test cases from assignment
</commit_message>
<xml_diff>
--- a/database/Projects_List.xlsx
+++ b/database/Projects_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/advait/Desktop/gitpositories/sc2002/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76BC3F5-0D6C-1141-9A5C-C2F959BFD1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89B4534-F688-D541-9617-313B8DB4FF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="5520" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="3160" windowWidth="23260" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,10 +123,10 @@
     <t>ReplacementSupervisor</t>
   </si>
   <si>
-    <t>AVAILABLE</t>
-  </si>
-  <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Available</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -505,13 +505,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -522,13 +522,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,13 +539,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -556,13 +556,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -573,13 +573,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -590,13 +590,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -607,13 +607,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -624,13 +624,13 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -641,13 +641,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -658,13 +658,13 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -675,13 +675,13 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -692,13 +692,13 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -709,13 +709,13 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -726,13 +726,13 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,13 +743,13 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -760,13 +760,13 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>